<commit_message>
the changes made according to the new data set
</commit_message>
<xml_diff>
--- a/DATA_SAMPLE_working_file_macedonia.xlsx
+++ b/DATA_SAMPLE_working_file_macedonia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb544155\OneDrive - WBG\Documents\GitHub\Microsimulation_Macedonia_Tax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{A29F52F4-D6C4-43C4-B14A-E28EC31A2605}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FC19291B-690F-460B-94ED-9C15888E94F7}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A29F52F4-D6C4-43C4-B14A-E28EC31A2605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2A9243E-7503-4BD9-B822-7397D6AF4DEF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="921" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -10470,10 +10472,10 @@
   <dimension ref="A1:W433"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10491,7 +10493,7 @@
     <col min="20" max="20" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="115.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>1955</v>
       </c>
@@ -33440,10 +33442,10 @@
   <dimension ref="A1:Q207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -61095,12 +61097,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61327,15 +61326,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404BF4E-48B7-4216-AC95-BFE7612BCEE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{599DF724-4924-414B-AD6F-BE1F9DAE29D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
+    <ds:schemaRef ds:uri="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -61360,18 +61371,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{599DF724-4924-414B-AD6F-BE1F9DAE29D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404BF4E-48B7-4216-AC95-BFE7612BCEE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
-    <ds:schemaRef ds:uri="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
made changes to the code
</commit_message>
<xml_diff>
--- a/DATA_SAMPLE_working_file_macedonia.xlsx
+++ b/DATA_SAMPLE_working_file_macedonia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb544155\OneDrive - WBG\Documents\GitHub\Microsimulation_Macedonia_Tax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/selahi_worldbank_org/Documents/Documents/GitHub/Microsimulation_Macedonia_Tax/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{A29F52F4-D6C4-43C4-B14A-E28EC31A2605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2A9243E-7503-4BD9-B822-7397D6AF4DEF}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A29F52F4-D6C4-43C4-B14A-E28EC31A2605}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97C84D1C-FCCE-4EFE-8B43-D0F9CCC701CC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="921" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="921" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pdd_gi_vidispid_c" sheetId="3" r:id="rId1"/>
@@ -6610,8 +6610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74F0785-18BD-4C92-9E44-C622255D7502}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7783,8 +7783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EF350D-5609-430F-8F32-6E862C8730E2}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9215,8 +9215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70D3086-D96B-4EAD-BADB-9F3A63A196FD}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9376,7 +9376,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G3" sqref="G3:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33442,10 +33442,10 @@
   <dimension ref="A1:Q207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="I198" sqref="I198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -44369,7 +44369,7 @@
   <dimension ref="A1:Q191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G3" sqref="G3:I191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54446,7 +54446,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G3" sqref="G3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54614,7 +54614,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="G3" sqref="G3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -54779,7 +54779,7 @@
   <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K96"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59820,8 +59820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BE3D2E-A728-4101-8A3F-73008DFF7F4D}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -61097,9 +61097,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61326,27 +61329,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{599DF724-4924-414B-AD6F-BE1F9DAE29D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404BF4E-48B7-4216-AC95-BFE7612BCEE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
-    <ds:schemaRef ds:uri="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -61371,9 +61362,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D404BF4E-48B7-4216-AC95-BFE7612BCEE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{599DF724-4924-414B-AD6F-BE1F9DAE29D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
+    <ds:schemaRef ds:uri="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>